<commit_message>
new: download dos dados e conversão de arquivos dbc para csv
</commit_message>
<xml_diff>
--- a/dicionarios/CNES/cnes_definicoes.xlsx
+++ b/dicionarios/CNES/cnes_definicoes.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ETL-ML-Dengue\dicionarios\CNES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Área de Trabalho\Pedro\Portifolio\ETL-ML-Dengue\dicionarios\CNES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC1C0F-E0DF-4EED-9EE8-492C5994CE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F0080F-4CE5-454A-955A-14C9DEA6ABF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A288F35F-5B18-4834-9965-1F5B4BB818BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A288F35F-5B18-4834-9965-1F5B4BB818BF}"/>
   </bookViews>
   <sheets>
     <sheet name="st" sheetId="1" r:id="rId1"/>
+    <sheet name="colunas_decodificar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="477">
   <si>
     <t>CNES</t>
   </si>
@@ -1840,18 +1841,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AA0F32-2328-46F8-8C19-C79B5C704683}">
   <dimension ref="A1:C237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:A79"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCellId="1" sqref="C1:C1048576 A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1928,7 +1929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1961,7 +1962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1994,7 +1995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2016,7 +2017,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2049,7 +2050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2082,7 +2083,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2148,7 +2149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -2170,7 +2171,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2192,7 +2193,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -2203,7 +2204,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -2214,7 +2215,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -2225,7 +2226,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -2313,7 +2314,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -2324,7 +2325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -2346,7 +2347,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -2368,7 +2369,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -2423,7 +2424,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -2434,7 +2435,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -2445,7 +2446,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -2456,7 +2457,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>112</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>116</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -2500,7 +2501,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -2522,7 +2523,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>128</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>130</v>
       </c>
@@ -2566,7 +2567,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>132</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -2599,7 +2600,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -2610,7 +2611,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>140</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>144</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>146</v>
       </c>
@@ -2654,7 +2655,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -2665,7 +2666,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -2676,7 +2677,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>152</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>154</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>156</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>158</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>160</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>166</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>170</v>
       </c>
@@ -2786,7 +2787,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>172</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>176</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -2830,7 +2831,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>182</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>184</v>
       </c>
@@ -2863,7 +2864,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>186</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>188</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>190</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>192</v>
       </c>
@@ -2907,7 +2908,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>194</v>
       </c>
@@ -2918,7 +2919,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>196</v>
       </c>
@@ -2929,7 +2930,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>198</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>200</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>202</v>
       </c>
@@ -2962,7 +2963,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>204</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>206</v>
       </c>
@@ -2984,7 +2985,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>208</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>210</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>212</v>
       </c>
@@ -3017,7 +3018,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>214</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>216</v>
       </c>
@@ -3039,7 +3040,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>218</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>220</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>224</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>226</v>
       </c>
@@ -3094,7 +3095,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>228</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>230</v>
       </c>
@@ -3116,7 +3117,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>232</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>234</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>236</v>
       </c>
@@ -3149,7 +3150,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>238</v>
       </c>
@@ -3160,7 +3161,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>240</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>242</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>244</v>
       </c>
@@ -3193,7 +3194,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>246</v>
       </c>
@@ -3204,7 +3205,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>248</v>
       </c>
@@ -3215,7 +3216,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>250</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>252</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>254</v>
       </c>
@@ -3248,7 +3249,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>256</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>258</v>
       </c>
@@ -3270,7 +3271,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>260</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>262</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>264</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>266</v>
       </c>
@@ -3314,7 +3315,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>268</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>270</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>272</v>
       </c>
@@ -3347,7 +3348,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>274</v>
       </c>
@@ -3358,7 +3359,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>276</v>
       </c>
@@ -3369,7 +3370,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>280</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>282</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>284</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>286</v>
       </c>
@@ -3424,7 +3425,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>288</v>
       </c>
@@ -3435,7 +3436,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>290</v>
       </c>
@@ -3446,7 +3447,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>292</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>294</v>
       </c>
@@ -3468,7 +3469,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>296</v>
       </c>
@@ -3479,7 +3480,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>298</v>
       </c>
@@ -3490,7 +3491,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>300</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>302</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>304</v>
       </c>
@@ -3523,7 +3524,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>306</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>308</v>
       </c>
@@ -3545,7 +3546,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>310</v>
       </c>
@@ -3556,7 +3557,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>312</v>
       </c>
@@ -3567,7 +3568,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>314</v>
       </c>
@@ -3578,7 +3579,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>316</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>318</v>
       </c>
@@ -3600,7 +3601,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>320</v>
       </c>
@@ -3611,7 +3612,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>322</v>
       </c>
@@ -3622,7 +3623,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>324</v>
       </c>
@@ -3633,7 +3634,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>326</v>
       </c>
@@ -3644,7 +3645,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>328</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>330</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>332</v>
       </c>
@@ -3677,7 +3678,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>334</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>336</v>
       </c>
@@ -3699,7 +3700,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>338</v>
       </c>
@@ -3710,7 +3711,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>340</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>342</v>
       </c>
@@ -3732,7 +3733,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>344</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>346</v>
       </c>
@@ -3754,7 +3755,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>348</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>350</v>
       </c>
@@ -3776,7 +3777,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>352</v>
       </c>
@@ -3787,7 +3788,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>354</v>
       </c>
@@ -3798,7 +3799,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -3809,7 +3810,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>358</v>
       </c>
@@ -3820,7 +3821,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>360</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>362</v>
       </c>
@@ -3842,7 +3843,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>364</v>
       </c>
@@ -3853,7 +3854,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>366</v>
       </c>
@@ -3864,7 +3865,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>368</v>
       </c>
@@ -3875,7 +3876,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>370</v>
       </c>
@@ -3886,7 +3887,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>372</v>
       </c>
@@ -3897,7 +3898,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>374</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>376</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>378</v>
       </c>
@@ -3930,7 +3931,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>380</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>382</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>384</v>
       </c>
@@ -3963,7 +3964,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>386</v>
       </c>
@@ -3974,7 +3975,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>388</v>
       </c>
@@ -3985,7 +3986,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>390</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>392</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>394</v>
       </c>
@@ -4018,7 +4019,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>396</v>
       </c>
@@ -4029,7 +4030,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>398</v>
       </c>
@@ -4040,7 +4041,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>400</v>
       </c>
@@ -4051,7 +4052,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>402</v>
       </c>
@@ -4062,7 +4063,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>404</v>
       </c>
@@ -4073,7 +4074,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>406</v>
       </c>
@@ -4084,7 +4085,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>408</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>410</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>412</v>
       </c>
@@ -4117,7 +4118,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>414</v>
       </c>
@@ -4128,7 +4129,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>416</v>
       </c>
@@ -4139,7 +4140,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>418</v>
       </c>
@@ -4150,7 +4151,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>420</v>
       </c>
@@ -4161,7 +4162,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>422</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>424</v>
       </c>
@@ -4183,7 +4184,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>426</v>
       </c>
@@ -4194,7 +4195,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>428</v>
       </c>
@@ -4205,7 +4206,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>430</v>
       </c>
@@ -4216,7 +4217,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>432</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>434</v>
       </c>
@@ -4238,7 +4239,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>436</v>
       </c>
@@ -4249,7 +4250,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>438</v>
       </c>
@@ -4260,7 +4261,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>440</v>
       </c>
@@ -4271,7 +4272,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>442</v>
       </c>
@@ -4282,7 +4283,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>444</v>
       </c>
@@ -4293,7 +4294,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>446</v>
       </c>
@@ -4304,7 +4305,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>448</v>
       </c>
@@ -4315,7 +4316,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>450</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>452</v>
       </c>
@@ -4337,7 +4338,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>454</v>
       </c>
@@ -4348,7 +4349,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>456</v>
       </c>
@@ -4359,7 +4360,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>458</v>
       </c>
@@ -4370,7 +4371,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>461</v>
       </c>
@@ -4381,7 +4382,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>463</v>
       </c>
@@ -4392,7 +4393,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>465</v>
       </c>
@@ -4403,7 +4404,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>467</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>469</v>
       </c>
@@ -4425,7 +4426,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>471</v>
       </c>
@@ -4436,7 +4437,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>473</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>475</v>
       </c>
@@ -4461,4 +4462,1000 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39FE035-B5D6-480F-9B17-453BF9678C3A}">
+  <dimension ref="A1:B122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>210</v>
+      </c>
+      <c r="B34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>218</v>
+      </c>
+      <c r="B35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>262</v>
+      </c>
+      <c r="B38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>264</v>
+      </c>
+      <c r="B39" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>266</v>
+      </c>
+      <c r="B40" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>268</v>
+      </c>
+      <c r="B41" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>270</v>
+      </c>
+      <c r="B42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>272</v>
+      </c>
+      <c r="B43" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>274</v>
+      </c>
+      <c r="B44" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>276</v>
+      </c>
+      <c r="B45" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>278</v>
+      </c>
+      <c r="B46" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>280</v>
+      </c>
+      <c r="B47" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>284</v>
+      </c>
+      <c r="B49" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>286</v>
+      </c>
+      <c r="B50" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>288</v>
+      </c>
+      <c r="B51" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>290</v>
+      </c>
+      <c r="B52" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>292</v>
+      </c>
+      <c r="B53" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>294</v>
+      </c>
+      <c r="B54" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>296</v>
+      </c>
+      <c r="B55" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>298</v>
+      </c>
+      <c r="B56" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>300</v>
+      </c>
+      <c r="B57" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>302</v>
+      </c>
+      <c r="B58" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>304</v>
+      </c>
+      <c r="B59" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>306</v>
+      </c>
+      <c r="B60" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>308</v>
+      </c>
+      <c r="B61" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>310</v>
+      </c>
+      <c r="B62" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>312</v>
+      </c>
+      <c r="B63" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>314</v>
+      </c>
+      <c r="B64" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>316</v>
+      </c>
+      <c r="B65" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>318</v>
+      </c>
+      <c r="B66" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>320</v>
+      </c>
+      <c r="B67" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>322</v>
+      </c>
+      <c r="B68" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>324</v>
+      </c>
+      <c r="B69" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>328</v>
+      </c>
+      <c r="B71" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>330</v>
+      </c>
+      <c r="B72" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>332</v>
+      </c>
+      <c r="B73" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>334</v>
+      </c>
+      <c r="B74" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>338</v>
+      </c>
+      <c r="B76" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>342</v>
+      </c>
+      <c r="B78" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>344</v>
+      </c>
+      <c r="B79" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>346</v>
+      </c>
+      <c r="B80" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>348</v>
+      </c>
+      <c r="B81" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>350</v>
+      </c>
+      <c r="B82" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>352</v>
+      </c>
+      <c r="B83" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>354</v>
+      </c>
+      <c r="B84" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>356</v>
+      </c>
+      <c r="B85" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>358</v>
+      </c>
+      <c r="B86" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>360</v>
+      </c>
+      <c r="B87" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>362</v>
+      </c>
+      <c r="B88" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>364</v>
+      </c>
+      <c r="B89" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>366</v>
+      </c>
+      <c r="B90" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>368</v>
+      </c>
+      <c r="B91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>370</v>
+      </c>
+      <c r="B92" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>372</v>
+      </c>
+      <c r="B93" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>374</v>
+      </c>
+      <c r="B94" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>376</v>
+      </c>
+      <c r="B95" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>378</v>
+      </c>
+      <c r="B96" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>380</v>
+      </c>
+      <c r="B97" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>382</v>
+      </c>
+      <c r="B98" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>384</v>
+      </c>
+      <c r="B99" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>386</v>
+      </c>
+      <c r="B100" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>388</v>
+      </c>
+      <c r="B101" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>390</v>
+      </c>
+      <c r="B102" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>392</v>
+      </c>
+      <c r="B103" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>394</v>
+      </c>
+      <c r="B104" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>396</v>
+      </c>
+      <c r="B105" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>398</v>
+      </c>
+      <c r="B106" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>400</v>
+      </c>
+      <c r="B107" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>402</v>
+      </c>
+      <c r="B108" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>404</v>
+      </c>
+      <c r="B109" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>406</v>
+      </c>
+      <c r="B110" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>408</v>
+      </c>
+      <c r="B111" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>410</v>
+      </c>
+      <c r="B112" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>412</v>
+      </c>
+      <c r="B113" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>414</v>
+      </c>
+      <c r="B114" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>416</v>
+      </c>
+      <c r="B115" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>418</v>
+      </c>
+      <c r="B116" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>420</v>
+      </c>
+      <c r="B117" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>422</v>
+      </c>
+      <c r="B118" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>424</v>
+      </c>
+      <c r="B119" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>426</v>
+      </c>
+      <c r="B120" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>428</v>
+      </c>
+      <c r="B121" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>430</v>
+      </c>
+      <c r="B122" t="s">
+        <v>431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>